<commit_message>
Add draw checking and artist stats
</commit_message>
<xml_diff>
--- a/EMSC-HoD-Country-Ranking.xlsx
+++ b/EMSC-HoD-Country-Ranking.xlsx
@@ -3740,7 +3740,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="203">
   <si>
     <t xml:space="preserve">HOD</t>
   </si>
@@ -4295,6 +4295,12 @@
   </si>
   <si>
     <t xml:space="preserve">Buraga Alexandru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toni Nikolov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joeri Groen</t>
   </si>
   <si>
     <t xml:space="preserve">EMSC-Country Statistics (after EMSC2202)</t>
@@ -6144,8 +6150,8 @@
   </sheetPr>
   <dimension ref="A1:BC1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L69" activeCellId="0" sqref="L69"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O77" activeCellId="0" sqref="O77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15507,6 +15513,16 @@
         <v>50</v>
       </c>
     </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G75" s="335" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G76" s="335" t="s">
+        <v>186</v>
+      </c>
+    </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -15545,31 +15561,31 @@
         <v>102</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="336" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B2" s="336"/>
       <c r="C2" s="336" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D2" s="336" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E2" s="336" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F2" s="336" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="G2" s="336" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H2" s="336" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15602,10 +15618,10 @@
         <v>1</v>
       </c>
       <c r="G4" s="336" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="H4" s="336" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="I4" s="335"/>
       <c r="J4" s="1" t="s">
@@ -15635,10 +15651,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="336" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="H5" s="336" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="I5" s="335"/>
     </row>
@@ -15662,10 +15678,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="336" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H6" s="336" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="I6" s="335"/>
     </row>
@@ -15689,7 +15705,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="336" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="H7" s="336"/>
       <c r="I7" s="335"/>
@@ -15714,7 +15730,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="336" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="H8" s="336"/>
       <c r="I8" s="335"/>
@@ -15739,7 +15755,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="336" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="H9" s="336"/>
       <c r="I9" s="335"/>
@@ -15764,7 +15780,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="336" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="H10" s="336"/>
       <c r="I10" s="335"/>
@@ -15812,7 +15828,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="336" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H12" s="336"/>
       <c r="I12" s="335"/>
@@ -15906,10 +15922,10 @@
         <v>0.86</v>
       </c>
       <c r="G16" s="336" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="H16" s="336" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15932,7 +15948,7 @@
         <v>0.86</v>
       </c>
       <c r="G17" s="336" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="H17" s="336"/>
       <c r="I17" s="335"/>
@@ -15957,7 +15973,7 @@
         <v>0.83</v>
       </c>
       <c r="G18" s="336" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="H18" s="336"/>
       <c r="I18" s="335"/>
@@ -15982,7 +15998,7 @@
         <v>0.83</v>
       </c>
       <c r="G19" s="336" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="H19" s="336"/>
       <c r="I19" s="335"/>
@@ -16007,7 +16023,7 @@
         <v>0.83</v>
       </c>
       <c r="G20" s="336" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H20" s="336"/>
       <c r="I20" s="335"/>
@@ -16032,7 +16048,7 @@
         <v>0.8</v>
       </c>
       <c r="G21" s="336" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="H21" s="336"/>
     </row>
@@ -16056,7 +16072,7 @@
         <v>0.8</v>
       </c>
       <c r="G22" s="336" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="H22" s="336"/>
       <c r="I22" s="335"/>
@@ -16104,7 +16120,7 @@
         <v>0.71</v>
       </c>
       <c r="G24" s="336" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="H24" s="336"/>
       <c r="I24" s="335"/>
@@ -16129,7 +16145,7 @@
         <v>0.71</v>
       </c>
       <c r="G25" s="336" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H25" s="336"/>
       <c r="I25" s="335"/>
@@ -16154,7 +16170,7 @@
         <v>0.71</v>
       </c>
       <c r="G26" s="336" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H26" s="336"/>
       <c r="I26" s="335"/>
@@ -16179,10 +16195,10 @@
         <v>0.67</v>
       </c>
       <c r="G27" s="336" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H27" s="336" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="I27" s="335"/>
     </row>
@@ -16206,10 +16222,10 @@
         <v>0.67</v>
       </c>
       <c r="G28" s="336" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H28" s="336" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="I28" s="335"/>
     </row>
@@ -16233,7 +16249,7 @@
         <v>0.67</v>
       </c>
       <c r="G29" s="336" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="H29" s="336"/>
       <c r="I29" s="335"/>
@@ -16303,7 +16319,7 @@
         <v>0.6</v>
       </c>
       <c r="G32" s="336" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H32" s="336"/>
       <c r="I32" s="335"/>
@@ -16328,10 +16344,10 @@
         <v>0.57</v>
       </c>
       <c r="G33" s="336" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="H33" s="336" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="I33" s="335"/>
     </row>
@@ -16355,7 +16371,7 @@
         <v>0.57</v>
       </c>
       <c r="G34" s="336" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="H34" s="336"/>
       <c r="I34" s="335"/>
@@ -16380,7 +16396,7 @@
         <v>0.57</v>
       </c>
       <c r="G35" s="336" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="H35" s="336"/>
       <c r="I35" s="335"/>
@@ -16405,7 +16421,7 @@
         <v>0.57</v>
       </c>
       <c r="G36" s="336" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H36" s="336"/>
       <c r="I36" s="335"/>
@@ -16430,7 +16446,7 @@
         <v>0.57</v>
       </c>
       <c r="G37" s="336" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H37" s="336"/>
       <c r="I37" s="335"/>
@@ -16455,7 +16471,7 @@
         <v>0.5</v>
       </c>
       <c r="G38" s="336" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="H38" s="336"/>
       <c r="I38" s="335"/>
@@ -16480,7 +16496,7 @@
         <v>0.5</v>
       </c>
       <c r="G39" s="336" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H39" s="336"/>
       <c r="I39" s="335"/>
@@ -16505,7 +16521,7 @@
         <v>0.5</v>
       </c>
       <c r="G40" s="336" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H40" s="336"/>
       <c r="I40" s="335"/>
@@ -16530,7 +16546,7 @@
         <v>0.5</v>
       </c>
       <c r="G41" s="336" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H41" s="336"/>
       <c r="I41" s="335"/>
@@ -16715,7 +16731,7 @@
         <v>0.29</v>
       </c>
       <c r="G49" s="336" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H49" s="336"/>
       <c r="I49" s="335"/>
@@ -16740,7 +16756,7 @@
         <v>0.25</v>
       </c>
       <c r="G50" s="336" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H50" s="336"/>
       <c r="I50" s="335"/>
@@ -16819,7 +16835,7 @@
         <v>50</v>
       </c>
       <c r="C54" s="336" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D54" s="336" t="n">
         <v>5</v>
@@ -16897,7 +16913,7 @@
       <c r="A58" s="336"/>
       <c r="B58" s="336"/>
       <c r="C58" s="336" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D58" s="336" t="n">
         <v>6</v>
@@ -16925,7 +16941,7 @@
       <c r="A60" s="336"/>
       <c r="B60" s="336"/>
       <c r="C60" s="336" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D60" s="336" t="n">
         <v>6</v>

</xml_diff>